<commit_message>
ajustes fase2 importar usuarios
</commit_message>
<xml_diff>
--- a/public/media/formato_usuarios.xlsx
+++ b/public/media/formato_usuarios.xlsx
@@ -11,7 +11,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
   <si>
     <t>Usuario</t>
   </si>
@@ -35,27 +35,6 @@
   </si>
   <si>
     <t>Supervisor</t>
-  </si>
-  <si>
-    <t>prueba</t>
-  </si>
-  <si>
-    <t>prueba@email.com</t>
-  </si>
-  <si>
-    <t>calle 3</t>
-  </si>
-  <si>
-    <t>prueba 2</t>
-  </si>
-  <si>
-    <t>prueba2</t>
-  </si>
-  <si>
-    <t>prueba2@email.com</t>
-  </si>
-  <si>
-    <t>calle 4</t>
   </si>
 </sst>
 </file>
@@ -166,57 +145,25 @@
       <c r="I1" s="2"/>
     </row>
     <row r="2" ht="15.75" customHeight="1">
-      <c r="A2" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="B2" s="3">
-        <v>12345.0</v>
-      </c>
-      <c r="C2" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="D2" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="E2" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="F2" s="3">
-        <v>12345.0</v>
-      </c>
-      <c r="G2" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="H2" s="3">
-        <v>1.0</v>
-      </c>
+      <c r="A2" s="3"/>
+      <c r="B2" s="3"/>
+      <c r="C2" s="3"/>
+      <c r="D2" s="3"/>
+      <c r="E2" s="3"/>
+      <c r="F2" s="3"/>
+      <c r="G2" s="3"/>
+      <c r="H2" s="3"/>
       <c r="I2" s="2"/>
     </row>
     <row r="3" ht="15.75" customHeight="1">
-      <c r="A3" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="B3" s="3">
-        <v>1234567.0</v>
-      </c>
-      <c r="C3" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="D3" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="E3" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="F3" s="3">
-        <v>1234567.0</v>
-      </c>
-      <c r="G3" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="H3" s="3">
-        <v>0.0</v>
-      </c>
+      <c r="A3" s="3"/>
+      <c r="B3" s="3"/>
+      <c r="C3" s="3"/>
+      <c r="D3" s="3"/>
+      <c r="E3" s="3"/>
+      <c r="F3" s="3"/>
+      <c r="G3" s="3"/>
+      <c r="H3" s="3"/>
       <c r="I3" s="2"/>
     </row>
   </sheetData>

</xml_diff>